<commit_message>
Poniendo imagenes en los Excel segun el Draw
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
+++ b/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/DOO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{190E16B6-2EFD-40E4-87AF-2CEF62795B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60FD0433-02F6-422B-9FED-BD6AE7093CC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3C9B1A-568B-470F-8836-C9DAC09531E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
   </bookViews>
@@ -2099,6 +2099,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2111,6 +2114,60 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2134,63 +2191,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2208,6 +2208,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38817</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54185A6A-4096-CC98-6392-B736D102E6F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="68580"/>
+          <a:ext cx="7772400" cy="3993597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2607,10 +2662,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="60"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2699,12 +2754,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2729,11 +2785,11 @@
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -2843,73 +2899,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="68" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>ConjuntoResidencial</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="69" t="str">
         <f>'[1]Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada uno de los residentes que son los que viven dentro de un conjunto residencial para generar reservas.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -3162,11 +3218,11 @@
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
@@ -3192,46 +3248,46 @@
     </row>
     <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70" t="s">
+      <c r="B14" s="74"/>
+      <c r="C14" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70" t="s">
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70" t="s">
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="70"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="70"/>
-      <c r="P14" s="70" t="s">
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="70"/>
-      <c r="R14" s="70" t="s">
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="S14" s="71"/>
+      <c r="S14" s="77"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="87"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="38" t="s">
         <v>69</v>
       </c>
@@ -3244,12 +3300,12 @@
       <c r="K15" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="72" t="s">
+      <c r="L15" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="76"/>
       <c r="P15" s="38" t="s">
         <v>71</v>
       </c>
@@ -3264,92 +3320,92 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="14"/>
       <c r="I16" s="12"/>
       <c r="J16" s="13"/>
       <c r="K16" s="12"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
       <c r="S16" s="40"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
       <c r="H17" s="43"/>
       <c r="I17" s="41"/>
       <c r="J17" s="42"/>
       <c r="K17" s="44"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="45"/>
       <c r="R17" s="45"/>
       <c r="S17" s="46"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
       <c r="H18" s="48"/>
       <c r="I18" s="49"/>
       <c r="J18" s="47"/>
       <c r="K18" s="50"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="84"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="84"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="51"/>
       <c r="R18" s="51"/>
       <c r="S18" s="52"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="H19" s="54"/>
       <c r="I19" s="55"/>
       <c r="J19" s="53"/>
       <c r="K19" s="54"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="88"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="56"/>
       <c r="R19" s="56"/>
@@ -3357,6 +3413,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="L16:O16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="L17:O17"/>
@@ -3369,17 +3436,6 @@
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="K14:O14"/>
     <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{68C0436B-E79D-44A7-88CE-82BDE933D82F}"/>
@@ -3436,73 +3492,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="68" t="str">
         <f>'[2]Listado Objetos de Dominio'!A5</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="69" t="str">
         <f>'[2]Listado Objetos de Dominio'!B5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -3830,14 +3886,14 @@
       <c r="U10" s="31"/>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="88"/>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="85"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -3863,46 +3919,46 @@
     </row>
     <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70" t="s">
+      <c r="B16" s="74"/>
+      <c r="C16" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70" t="s">
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70" t="s">
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="S16" s="71"/>
+      <c r="S16" s="77"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="87"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
       <c r="H17" s="38" t="s">
         <v>69</v>
       </c>
@@ -3915,12 +3971,12 @@
       <c r="K17" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="72" t="s">
+      <c r="L17" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="76"/>
+      <c r="O17" s="76"/>
       <c r="P17" s="38" t="s">
         <v>71</v>
       </c>
@@ -3935,92 +3991,92 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="14"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="40"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="43"/>
       <c r="I19" s="41"/>
       <c r="J19" s="42"/>
       <c r="K19" s="44"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="45"/>
       <c r="R19" s="45"/>
       <c r="S19" s="46"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
       <c r="H20" s="48"/>
       <c r="I20" s="49"/>
       <c r="J20" s="47"/>
       <c r="K20" s="50"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="51"/>
       <c r="R20" s="51"/>
       <c r="S20" s="52"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="H21" s="54"/>
       <c r="I21" s="55"/>
       <c r="J21" s="53"/>
       <c r="K21" s="54"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="88"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="56"/>
       <c r="R21" s="56"/>
@@ -4028,17 +4084,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="L19:O19"/>
@@ -4051,6 +4096,17 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:O16"/>
     <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B8FCC087-AC99-4C6B-BC9A-E2AC36CAED41}"/>
@@ -4107,73 +4163,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="68" t="str">
         <f>'Listado Objetos de Dominio'!A5</f>
         <v>TipoZonaComun</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="69" t="str">
         <f>'Listado Objetos de Dominio'!B5</f>
         <v xml:space="preserve"> Objeto de dominio que representa las categorías o tipos de zonas comunes disponibles en un conjunto residencial.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -4382,14 +4438,14 @@
       <c r="U7" s="31"/>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="88"/>
+      <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="72"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
@@ -4415,46 +4471,46 @@
     </row>
     <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70" t="s">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70" t="s">
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70" t="s">
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="L13" s="70"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="70" t="s">
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70" t="s">
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="S13" s="71"/>
+      <c r="S13" s="77"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="87"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="38" t="s">
         <v>69</v>
       </c>
@@ -4467,12 +4523,12 @@
       <c r="K14" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="76"/>
+      <c r="O14" s="76"/>
       <c r="P14" s="38" t="s">
         <v>71</v>
       </c>
@@ -4487,92 +4543,92 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="14"/>
       <c r="I15" s="12"/>
       <c r="J15" s="13"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="S15" s="40"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="43"/>
       <c r="I16" s="41"/>
       <c r="J16" s="42"/>
       <c r="K16" s="44"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="45"/>
       <c r="S16" s="46"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
       <c r="H17" s="48"/>
       <c r="I17" s="49"/>
       <c r="J17" s="47"/>
       <c r="K17" s="50"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="65"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
       <c r="P17" s="30"/>
       <c r="Q17" s="51"/>
       <c r="R17" s="51"/>
       <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="H18" s="54"/>
       <c r="I18" s="55"/>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
+      <c r="O18" s="88"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="56"/>
       <c r="R18" s="56"/>
@@ -4580,17 +4636,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="L15:O15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="L16:O16"/>
@@ -4603,6 +4648,17 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="K13:O13"/>
     <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{0E7B0C62-6DE1-4F39-948B-B7E7FB6516CF}"/>

</xml_diff>

<commit_message>
Termine la relacion Reserva-0002
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
+++ b/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250871BC-7344-445D-B911-2C2D8A1DE7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D246396-BE61-45F3-B54E-2B9F9E842340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="4" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -1332,7 +1332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="89">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1589,13 +1589,16 @@
     <t>identificador unico de zona comun</t>
   </si>
   <si>
-    <t>idTipoZonaComun</t>
-  </si>
-  <si>
     <t>TipoZonaComun</t>
   </si>
   <si>
     <t>No es posible tener más de un tipo de  zona común con el mismo numero de identificación.</t>
+  </si>
+  <si>
+    <t>conjuntoResidencial</t>
+  </si>
+  <si>
+    <t>tipoZonaComun</t>
   </si>
 </sst>
 </file>
@@ -2279,8 +2282,8 @@
       <sheetName val="ZonaComun"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="5">
           <cell r="A5" t="str">
@@ -2291,9 +2294,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2622,19 +2625,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="61"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2650,7 +2653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2658,52 +2661,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2724,7 +2727,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2739,16 +2742,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="8"/>
+    <col min="1" max="1" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2758,7 +2761,7 @@
       <c r="C1" s="62"/>
       <c r="D1" s="63"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>Administración conjunto residencial</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>Administración conjunto residencial</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="str">
         <f>"TipoZonaComun"</f>
         <v>TipoZonaComun</v>
@@ -2838,34 +2841,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>25</v>
       </c>
@@ -2886,7 +2889,7 @@
       <c r="P1" s="68"/>
       <c r="Q1" s="68"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
@@ -2910,7 +2913,7 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -2934,7 +2937,7 @@
       <c r="P3" s="70"/>
       <c r="Q3" s="70"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>44</v>
       </c>
@@ -3048,7 +3051,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
@@ -3095,7 +3098,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>71</v>
       </c>
@@ -3140,15 +3143,15 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="73"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>55</v>
       </c>
@@ -3159,7 +3162,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="59" t="s">
         <v>82</v>
       </c>
@@ -3170,8 +3173,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>57</v>
       </c>
@@ -3204,7 +3207,7 @@
       </c>
       <c r="S13" s="78"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="76"/>
       <c r="B14" s="77"/>
       <c r="C14" s="77"/>
@@ -3243,7 +3246,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>67</v>
       </c>
@@ -3266,7 +3269,7 @@
       <c r="R15" s="14"/>
       <c r="S15" s="40"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>68</v>
       </c>
@@ -3289,7 +3292,7 @@
       <c r="R16" s="45"/>
       <c r="S16" s="46"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="82" t="s">
         <v>69</v>
       </c>
@@ -3312,7 +3315,7 @@
       <c r="R17" s="51"/>
       <c r="S17" s="52"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="86" t="s">
         <v>70</v>
       </c>
@@ -3382,40 +3385,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC94481-E3CC-43E3-941E-02D7E4865B6C}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>25</v>
       </c>
@@ -3436,7 +3439,7 @@
       <c r="P1" s="68"/>
       <c r="Q1" s="68"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
@@ -3460,7 +3463,7 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -3484,7 +3487,7 @@
       <c r="P3" s="70"/>
       <c r="Q3" s="70"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -3537,23 +3540,23 @@
         <v>2</v>
       </c>
       <c r="R4" s="19" t="str">
-        <f>A16</f>
+        <f>A17</f>
         <v>Reponsabilidad 1</v>
       </c>
       <c r="S4" s="20" t="str">
-        <f>A17</f>
+        <f>A18</f>
         <v>Reponsabilidad 2</v>
       </c>
       <c r="T4" s="21" t="str">
-        <f>A18</f>
+        <f>A19</f>
         <v>Reponsabilidad 3</v>
       </c>
       <c r="U4" s="22" t="str">
-        <f>A19</f>
+        <f>A20</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>44</v>
       </c>
@@ -3598,7 +3601,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
@@ -3645,7 +3648,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>77</v>
       </c>
@@ -3686,12 +3689,12 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -3713,242 +3716,269 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="58"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="71" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="58"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="B11" s="72"/>
+      <c r="C11" s="73"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B12" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C12" s="34" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="59" t="s">
+    <row r="13" spans="1:21" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C13" s="37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75" t="s">
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75" t="s">
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="75"/>
-      <c r="P14" s="75" t="s">
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75" t="s">
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="S14" s="78"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="76"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="38" t="s">
+      <c r="S15" s="78"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I16" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="77" t="s">
+      <c r="L16" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="38" t="s">
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q15" s="38" t="s">
+      <c r="Q16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="R15" s="38" t="s">
+      <c r="R16" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="S15" s="39" t="s">
+      <c r="S16" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="79" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="40"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="B17" s="80"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="40"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="67"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="46"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="82" t="s">
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="46"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="52"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="86" t="s">
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="52"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="89"/>
-      <c r="M19" s="89"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="57"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:G16"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="L16:O16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B8FCC087-AC99-4C6B-BC9A-E2AC36CAED41}"/>
-    <hyperlink ref="I19" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{CDF51FA1-95E8-458D-B08D-DE6B83D11E90}"/>
+    <hyperlink ref="I20" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{CDF51FA1-95E8-458D-B08D-DE6B83D11E90}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{E8AED8A1-D46F-4E6A-A688-B030C913C178}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{5204543D-2FD3-4C52-A214-40DAFC4AB330}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{24B0CFBA-B422-4BB7-8C7F-510DDC30BE26}"/>
-    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C597EA1C-A221-4684-B293-242B3F8A541E}"/>
-    <hyperlink ref="A16:B16" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{56C317F9-9561-44AC-B9C2-329CFDD0A0FD}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{D41B6581-A976-442C-B954-5594B5BDBAE4}"/>
+    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C597EA1C-A221-4684-B293-242B3F8A541E}"/>
+    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{56C317F9-9561-44AC-B9C2-329CFDD0A0FD}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{D41B6581-A976-442C-B954-5594B5BDBAE4}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{307E0460-9076-4914-963A-10FAC8B6A64E}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{E29D6D57-D115-4134-897D-1A336068BAFD}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{832DA90C-BACA-4EC2-B66D-D2764CD09DA1}"/>
-    <hyperlink ref="C12" location="ZonaComun!A8" display="identificador" xr:uid="{80372D6B-38D9-46D9-A913-E7AC275EFEAE}"/>
+    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{832DA90C-BACA-4EC2-B66D-D2764CD09DA1}"/>
+    <hyperlink ref="C13" location="ZonaComun!A8" display="identificador" xr:uid="{80372D6B-38D9-46D9-A913-E7AC275EFEAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3959,38 +3989,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD40DA5A-DF0C-47D3-BDA3-0E9F4D55D663}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>25</v>
       </c>
@@ -4011,7 +4041,7 @@
       <c r="P1" s="68"/>
       <c r="Q1" s="68"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
@@ -4035,7 +4065,7 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -4059,7 +4089,7 @@
       <c r="P3" s="70"/>
       <c r="Q3" s="70"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -4128,7 +4158,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>44</v>
       </c>
@@ -4173,7 +4203,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>50</v>
       </c>
@@ -4220,17 +4250,17 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="71" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="73"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>55</v>
       </c>
@@ -4241,19 +4271,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>57</v>
       </c>
@@ -4286,7 +4316,7 @@
       </c>
       <c r="S12" s="78"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="76"/>
       <c r="B13" s="77"/>
       <c r="C13" s="77"/>
@@ -4325,7 +4355,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>67</v>
       </c>
@@ -4348,7 +4378,7 @@
       <c r="R14" s="14"/>
       <c r="S14" s="40"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>68</v>
       </c>
@@ -4371,7 +4401,7 @@
       <c r="R15" s="45"/>
       <c r="S15" s="46"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="82" t="s">
         <v>69</v>
       </c>
@@ -4394,7 +4424,7 @@
       <c r="R16" s="51"/>
       <c r="S16" s="52"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="86" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Creando Carpeta seccion 7 donde empezamos con la nueva parte de event storming
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
+++ b/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquesido Conjuntos Residenciales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D246396-BE61-45F3-B54E-2B9F9E842340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C15037-D39D-4FB8-A295-43FFEA05B278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="4" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -2084,6 +2084,48 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2117,50 +2159,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2738,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691F8BFD-AB91-4BB3-AD21-0479D3D78DFA}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,73 +2869,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="83" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>ConjuntoResidencial</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="70" t="str">
+      <c r="B3" s="84" t="str">
         <f>'[1]Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada uno de los residentes que son los que viven dentro de un conjunto residencial para generar reservas.</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -3145,11 +3145,11 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="87"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
@@ -3175,46 +3175,46 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75" t="s">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75" t="s">
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75" t="s">
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75" t="s">
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75" t="s">
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="S13" s="78"/>
+      <c r="S13" s="73"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
       <c r="H14" s="38" t="s">
         <v>62</v>
       </c>
@@ -3227,12 +3227,12 @@
       <c r="K14" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="77" t="s">
+      <c r="L14" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
       <c r="P14" s="38" t="s">
         <v>64</v>
       </c>
@@ -3247,92 +3247,92 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="14"/>
       <c r="I15" s="12"/>
       <c r="J15" s="13"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="S15" s="40"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="43"/>
       <c r="I16" s="41"/>
       <c r="J16" s="42"/>
       <c r="K16" s="44"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="45"/>
       <c r="S16" s="46"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="48"/>
       <c r="I17" s="49"/>
       <c r="J17" s="47"/>
       <c r="K17" s="50"/>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
       <c r="P17" s="30"/>
       <c r="Q17" s="51"/>
       <c r="R17" s="51"/>
       <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="54"/>
       <c r="I18" s="55"/>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="89"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="89"/>
-      <c r="O18" s="89"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="71"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="56"/>
       <c r="R18" s="56"/>
@@ -3340,17 +3340,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="L15:O15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="L16:O16"/>
@@ -3363,6 +3352,17 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="K13:O13"/>
     <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{68C0436B-E79D-44A7-88CE-82BDE933D82F}"/>
@@ -3387,7 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC94481-E3CC-43E3-941E-02D7E4865B6C}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3419,73 +3419,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="83" t="str">
         <f>'[2]Listado Objetos de Dominio'!A5</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="70" t="str">
+      <c r="B3" s="84" t="str">
         <f>'[2]Listado Objetos de Dominio'!B5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -3747,11 +3747,11 @@
       <c r="D10" s="58"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="87"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
@@ -3777,46 +3777,46 @@
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75" t="s">
+      <c r="B15" s="72"/>
+      <c r="C15" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75" t="s">
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75" t="s">
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="75" t="s">
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75" t="s">
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="S15" s="78"/>
+      <c r="S15" s="73"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
       <c r="H16" s="38" t="s">
         <v>62</v>
       </c>
@@ -3829,12 +3829,12 @@
       <c r="K16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="77" t="s">
+      <c r="L16" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
       <c r="P16" s="38" t="s">
         <v>64</v>
       </c>
@@ -3849,92 +3849,92 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
       <c r="H17" s="14"/>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="40"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
       <c r="H18" s="43"/>
       <c r="I18" s="41"/>
       <c r="J18" s="42"/>
       <c r="K18" s="44"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="67"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="45"/>
       <c r="R18" s="45"/>
       <c r="S18" s="46"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
       <c r="H19" s="48"/>
       <c r="I19" s="49"/>
       <c r="J19" s="47"/>
       <c r="K19" s="50"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="51"/>
       <c r="R19" s="51"/>
       <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="87"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="54"/>
       <c r="I20" s="55"/>
       <c r="J20" s="53"/>
       <c r="K20" s="54"/>
-      <c r="L20" s="89"/>
-      <c r="M20" s="89"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="89"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="56"/>
       <c r="R20" s="56"/>
@@ -3942,6 +3942,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="L18:O18"/>
@@ -3954,17 +3965,6 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="K15:O15"/>
     <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B8FCC087-AC99-4C6B-BC9A-E2AC36CAED41}"/>
@@ -4021,73 +4021,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="83" t="str">
         <f>'Listado Objetos de Dominio'!A5</f>
         <v>TipoZonaComun</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="70" t="str">
+      <c r="B3" s="84" t="str">
         <f>'Listado Objetos de Dominio'!B5</f>
         <v xml:space="preserve"> Objeto de dominio que representa las categorías o tipos de zonas comunes disponibles en un conjunto residencial.</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -4254,11 +4254,11 @@
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="73"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="87"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
@@ -4284,46 +4284,46 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75" t="s">
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75" t="s">
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75" t="s">
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75" t="s">
+      <c r="Q12" s="72"/>
+      <c r="R12" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="S12" s="78"/>
+      <c r="S12" s="73"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
       <c r="H13" s="38" t="s">
         <v>62</v>
       </c>
@@ -4336,12 +4336,12 @@
       <c r="K13" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L13" s="77" t="s">
+      <c r="L13" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
       <c r="P13" s="38" t="s">
         <v>64</v>
       </c>
@@ -4356,92 +4356,92 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="14"/>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="S14" s="40"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="43"/>
       <c r="I15" s="41"/>
       <c r="J15" s="42"/>
       <c r="K15" s="44"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="45"/>
       <c r="S15" s="46"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
       <c r="H16" s="48"/>
       <c r="I16" s="49"/>
       <c r="J16" s="47"/>
       <c r="K16" s="50"/>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
       <c r="P16" s="30"/>
       <c r="Q16" s="51"/>
       <c r="R16" s="51"/>
       <c r="S16" s="52"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="54"/>
       <c r="I17" s="55"/>
       <c r="J17" s="53"/>
       <c r="K17" s="54"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="89"/>
-      <c r="O17" s="89"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
       <c r="P17" s="31"/>
       <c r="Q17" s="56"/>
       <c r="R17" s="56"/>
@@ -4449,6 +4449,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="L14:O14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="L15:O15"/>
@@ -4461,17 +4472,6 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:O12"/>
     <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{0E7B0C62-6DE1-4F39-948B-B7E7FB6516CF}"/>

</xml_diff>